<commit_message>
Testing file added, tqdm deleted (all functions wrok silently now)
</commit_message>
<xml_diff>
--- a/tests/TEST_config_file.xlsx
+++ b/tests/TEST_config_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\Desktop\CLIP_database_project\Database_comparator\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E66BE5-7069-4F92-90AF-3022B26B2907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62902907-6082-44B9-9446-6169902192D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query" sheetId="1" r:id="rId1"/>
@@ -1301,7 +1301,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1363,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1377,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="14">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>